<commit_message>
Variance Analysis of Q1 and Q2 Year-Over-Year
</commit_message>
<xml_diff>
--- a/Volume by Region Data Request v2.xlsx
+++ b/Volume by Region Data Request v2.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sahil\Documents\Github\excelprogress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E6EB53-8FB7-458F-90E5-C0C601368D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52FC2FA-981F-4238-A455-DAA5FB43358D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" tabRatio="458" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3043" uniqueCount="932">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3065" uniqueCount="936">
   <si>
     <t>CLID</t>
   </si>
@@ -2863,15 +2863,28 @@
   </si>
   <si>
     <t>Sum of Vol</t>
+  </si>
+  <si>
+    <t>Q1 YoY</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Q2 YoY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="172" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -2912,14 +2925,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -2933,21 +2947,31 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Text UPPER lower" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="150">
+  <dxfs count="162">
     <dxf>
       <alignment wrapText="0"/>
     </dxf>
@@ -3129,7 +3153,37 @@
       <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -3168,10 +3222,7 @@
       <alignment wrapText="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <alignment wrapText="0"/>
@@ -3207,7 +3258,7 @@
       <alignment wrapText="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <alignment wrapText="0"/>
@@ -3243,7 +3294,7 @@
       <alignment wrapText="0"/>
     </dxf>
     <dxf>
-      <alignment wrapText="0"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <alignment wrapText="0"/>
@@ -3279,34 +3330,7 @@
       <alignment wrapText="0"/>
     </dxf>
     <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -3431,6 +3455,42 @@
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -3513,6 +3573,1791 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Volume by Region Data Request v2.xlsx]Pivot!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Pivot!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NAM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Pivot!$A$5:$A$13</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Qtr3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Qtr4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2020</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2021</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Pivot!$B$5:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>509419</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>576618</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>363694</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>432034</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>530019</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>596502</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4CC4-4D8A-B91B-6CD75006F8EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Pivot!$C$3:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EMEA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Pivot!$A$5:$A$13</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Qtr3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Qtr4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2020</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2021</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Pivot!$C$5:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>147852</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>173566</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>103536</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>129264</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150204</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>176338</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4CC4-4D8A-B91B-6CD75006F8EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Pivot!$D$3:$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>APAC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Pivot!$A$5:$A$13</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Qtr3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Qtr4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2020</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2021</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Pivot!$D$5:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>95736</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>107338</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69198</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80144</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99778</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>109811</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4CC4-4D8A-B91B-6CD75006F8EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Pivot!$E$3:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LATAM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Pivot!$A$5:$A$13</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Qtr3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Qtr4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2020</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2021</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Pivot!$E$5:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>69053</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82618</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50574</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75265</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82631</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-4CC4-4D8A-B91B-6CD75006F8EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2002302095"/>
+        <c:axId val="2002302511"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2002302095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2002302511"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2002302511"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2002302095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F63985D6-D8A4-4A61-9579-39D8210CA882}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12704,11 +14549,11 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D37C5FD1-A12E-4EA3-A67C-2BFE15959C89}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:G11" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B3596AE5-7ABE-4BFD-935E-B17364891890}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A33:G40" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisCol" numFmtId="14" showAll="0" defaultSubtotal="0">
+    <pivotField numFmtId="14" showAll="0" defaultSubtotal="0">
       <items count="14">
         <item x="0"/>
         <item x="1"/>
@@ -12759,12 +14604,12 @@
     <pivotField showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
       <items count="6">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
       </items>
     </pivotField>
     <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
@@ -12796,10 +14641,9 @@
       <x/>
     </i>
   </rowItems>
-  <colFields count="3">
+  <colFields count="2">
     <field x="9"/>
     <field x="8"/>
-    <field x="1"/>
   </colFields>
   <colItems count="6">
     <i>
@@ -12827,38 +14671,38 @@
     <dataField name="Sum of Vol" fld="2" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="12">
-    <format dxfId="119">
+    <format dxfId="60">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="118">
+    <format dxfId="61">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="117">
+    <format dxfId="62">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="116">
+    <format dxfId="63">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="115">
+    <format dxfId="64">
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="114">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="2"/>
+    <format dxfId="65">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="113">
+    <format dxfId="66">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="112">
+    <format dxfId="67">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="111">
+    <format dxfId="68">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="110">
+    <format dxfId="69">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="2">
@@ -12868,13 +14712,481 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="109">
+    <format dxfId="70">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="61">
+    <format dxfId="71">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
+  <chartFormats count="10">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D37C5FD1-A12E-4EA3-A67C-2BFE15959C89}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:E13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" numFmtId="14" showAll="0" defaultSubtotal="0">
+      <items count="14">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="164" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisCol" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="4">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item sd="0" x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item sd="0" x="3"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="9"/>
+    <field x="8"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="5"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Vol" fld="2" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <formats count="12">
+    <format dxfId="161">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="160">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="159">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="158">
+      <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="157">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="156">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
+    </format>
+    <format dxfId="155">
+      <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="154">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="5" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="153">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="152">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="9" count="2">
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="151">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="150">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="10">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -13300,150 +15612,150 @@
   <sheetFormatPr defaultRowHeight="13.15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>897</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -21755,221 +24067,1075 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472D7B1D-3022-458C-99D2-1C6B8FA100F0}">
-  <dimension ref="A3:J11"/>
+  <dimension ref="A3:Y61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="3" customWidth="1"/>
+    <col min="11" max="13" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="25" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="26" max="27" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="29" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>931</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>924</v>
       </c>
+      <c r="F3"/>
+      <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
       <c r="J3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>922</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>925</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>926</v>
-      </c>
+        <v>898</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>908</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>907</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4"/>
       <c r="H4"/>
       <c r="I4"/>
       <c r="J4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
-        <v>927</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>928</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>929</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>930</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>927</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>928</v>
-      </c>
+      <c r="A5" s="8" t="s">
+        <v>925</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5"/>
+      <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>922</v>
-      </c>
+      <c r="A6" s="12" t="s">
+        <v>927</v>
+      </c>
+      <c r="B6" s="9">
+        <v>509419</v>
+      </c>
+      <c r="C6" s="9">
+        <v>147852</v>
+      </c>
+      <c r="D6" s="9">
+        <v>95736</v>
+      </c>
+      <c r="E6" s="9">
+        <v>69053</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6"/>
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>898</v>
-      </c>
-      <c r="B7" s="10">
-        <v>509419</v>
-      </c>
-      <c r="C7" s="10">
+      <c r="A7" s="12" t="s">
+        <v>928</v>
+      </c>
+      <c r="B7" s="9">
         <v>576618</v>
       </c>
-      <c r="D7" s="10">
-        <v>363694</v>
-      </c>
-      <c r="E7" s="10">
-        <v>432034</v>
-      </c>
-      <c r="F7" s="10">
-        <v>530019</v>
-      </c>
-      <c r="G7" s="10">
-        <v>596502</v>
-      </c>
+      <c r="C7" s="9">
+        <v>173566</v>
+      </c>
+      <c r="D7" s="9">
+        <v>107338</v>
+      </c>
+      <c r="E7" s="9">
+        <v>82618</v>
+      </c>
+      <c r="F7"/>
+      <c r="G7"/>
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>899</v>
-      </c>
-      <c r="B8" s="10">
-        <v>147852</v>
-      </c>
-      <c r="C8" s="10">
-        <v>173566</v>
-      </c>
-      <c r="D8" s="10">
+      <c r="A8" s="12" t="s">
+        <v>929</v>
+      </c>
+      <c r="B8" s="9">
+        <v>363694</v>
+      </c>
+      <c r="C8" s="9">
         <v>103536</v>
       </c>
-      <c r="E8" s="10">
-        <v>129264</v>
-      </c>
-      <c r="F8" s="10">
-        <v>150204</v>
-      </c>
-      <c r="G8" s="10">
-        <v>176338</v>
-      </c>
+      <c r="D8" s="9">
+        <v>69198</v>
+      </c>
+      <c r="E8" s="9">
+        <v>50574</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8"/>
       <c r="H8"/>
       <c r="I8"/>
       <c r="J8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>908</v>
-      </c>
-      <c r="B9" s="10">
-        <v>95736</v>
-      </c>
-      <c r="C9" s="10">
-        <v>107338</v>
-      </c>
-      <c r="D9" s="10">
-        <v>69198</v>
-      </c>
-      <c r="E9" s="10">
+      <c r="A9" s="12" t="s">
+        <v>930</v>
+      </c>
+      <c r="B9" s="9">
+        <v>432034</v>
+      </c>
+      <c r="C9" s="9">
+        <v>129264</v>
+      </c>
+      <c r="D9" s="9">
         <v>80144</v>
       </c>
-      <c r="F9" s="10">
-        <v>99778</v>
-      </c>
-      <c r="G9" s="10">
-        <v>109811</v>
-      </c>
+      <c r="E9" s="9">
+        <v>65121</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9"/>
       <c r="H9"/>
       <c r="I9"/>
       <c r="J9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>907</v>
-      </c>
-      <c r="B10" s="10">
-        <v>69053</v>
-      </c>
-      <c r="C10" s="10">
-        <v>82618</v>
-      </c>
-      <c r="D10" s="10">
-        <v>50574</v>
-      </c>
-      <c r="E10" s="10">
-        <v>65121</v>
-      </c>
-      <c r="F10" s="10">
-        <v>75265</v>
-      </c>
-      <c r="G10" s="10">
-        <v>82631</v>
-      </c>
+      <c r="A10" s="8" t="s">
+        <v>926</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10"/>
+      <c r="G10"/>
       <c r="H10"/>
       <c r="I10"/>
       <c r="J10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
-        <v>923</v>
-      </c>
-      <c r="B11" s="10">
-        <v>822060</v>
-      </c>
-      <c r="C11" s="10">
-        <v>940140</v>
-      </c>
-      <c r="D11" s="10">
-        <v>587002</v>
-      </c>
-      <c r="E11" s="10">
-        <v>706563</v>
-      </c>
-      <c r="F11" s="10">
-        <v>855266</v>
-      </c>
-      <c r="G11" s="10">
-        <v>965282</v>
-      </c>
+      <c r="A11" s="12" t="s">
+        <v>927</v>
+      </c>
+      <c r="B11" s="9">
+        <v>530019</v>
+      </c>
+      <c r="C11" s="9">
+        <v>150204</v>
+      </c>
+      <c r="D11" s="9">
+        <v>99778</v>
+      </c>
+      <c r="E11" s="9">
+        <v>75265</v>
+      </c>
+      <c r="F11"/>
+      <c r="G11"/>
       <c r="H11"/>
       <c r="I11"/>
       <c r="J11"/>
     </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>928</v>
+      </c>
+      <c r="B12" s="9">
+        <v>596502</v>
+      </c>
+      <c r="C12" s="9">
+        <v>176338</v>
+      </c>
+      <c r="D12" s="9">
+        <v>109811</v>
+      </c>
+      <c r="E12" s="9">
+        <v>82631</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>923</v>
+      </c>
+      <c r="B13" s="9">
+        <v>3008286</v>
+      </c>
+      <c r="C13" s="9">
+        <v>880760</v>
+      </c>
+      <c r="D13" s="9">
+        <v>562005</v>
+      </c>
+      <c r="E13" s="9">
+        <v>425262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>931</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>924</v>
+      </c>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+      <c r="T33"/>
+      <c r="U33"/>
+      <c r="V33"/>
+      <c r="W33"/>
+      <c r="X33"/>
+      <c r="Y33"/>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
+        <v>925</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>926</v>
+      </c>
+      <c r="H34"/>
+      <c r="I34" s="3" t="s">
+        <v>932</v>
+      </c>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34" t="s">
+        <v>935</v>
+      </c>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
+      <c r="Y34"/>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>922</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>927</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>928</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>929</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>930</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>927</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>928</v>
+      </c>
+      <c r="H35"/>
+      <c r="I35" s="3" t="s">
+        <v>933</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>934</v>
+      </c>
+      <c r="K35"/>
+      <c r="L35" s="3" t="s">
+        <v>933</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>934</v>
+      </c>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>898</v>
+      </c>
+      <c r="B36" s="9">
+        <v>509419</v>
+      </c>
+      <c r="C36" s="9">
+        <v>576618</v>
+      </c>
+      <c r="D36" s="9">
+        <v>363694</v>
+      </c>
+      <c r="E36" s="9">
+        <v>432034</v>
+      </c>
+      <c r="F36" s="9">
+        <v>530019</v>
+      </c>
+      <c r="G36" s="9">
+        <v>596502</v>
+      </c>
+      <c r="H36"/>
+      <c r="I36" s="11">
+        <f>F36-B36</f>
+        <v>20600</v>
+      </c>
+      <c r="J36" s="13">
+        <f>F36/B36-1</f>
+        <v>4.0438224722674221E-2</v>
+      </c>
+      <c r="K36"/>
+      <c r="L36" s="11">
+        <f>G36-C36</f>
+        <v>19884</v>
+      </c>
+      <c r="M36" s="13">
+        <f>G36/C36-1</f>
+        <v>3.4483835051975387E-2</v>
+      </c>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>899</v>
+      </c>
+      <c r="B37" s="9">
+        <v>147852</v>
+      </c>
+      <c r="C37" s="9">
+        <v>173566</v>
+      </c>
+      <c r="D37" s="9">
+        <v>103536</v>
+      </c>
+      <c r="E37" s="9">
+        <v>129264</v>
+      </c>
+      <c r="F37" s="9">
+        <v>150204</v>
+      </c>
+      <c r="G37" s="9">
+        <v>176338</v>
+      </c>
+      <c r="H37"/>
+      <c r="I37" s="11">
+        <f t="shared" ref="I37:I40" si="0">F37-B37</f>
+        <v>2352</v>
+      </c>
+      <c r="J37" s="13">
+        <f t="shared" ref="J37:J40" si="1">F37/B37-1</f>
+        <v>1.5907799691583513E-2</v>
+      </c>
+      <c r="K37"/>
+      <c r="L37" s="11">
+        <f t="shared" ref="L37:L40" si="2">G37-C37</f>
+        <v>2772</v>
+      </c>
+      <c r="M37" s="13">
+        <f t="shared" ref="M37:M40" si="3">G37/C37-1</f>
+        <v>1.5970869870827187E-2</v>
+      </c>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>908</v>
+      </c>
+      <c r="B38" s="9">
+        <v>95736</v>
+      </c>
+      <c r="C38" s="9">
+        <v>107338</v>
+      </c>
+      <c r="D38" s="9">
+        <v>69198</v>
+      </c>
+      <c r="E38" s="9">
+        <v>80144</v>
+      </c>
+      <c r="F38" s="9">
+        <v>99778</v>
+      </c>
+      <c r="G38" s="9">
+        <v>109811</v>
+      </c>
+      <c r="H38"/>
+      <c r="I38" s="11">
+        <f t="shared" si="0"/>
+        <v>4042</v>
+      </c>
+      <c r="J38" s="13">
+        <f t="shared" si="1"/>
+        <v>4.2220272415810056E-2</v>
+      </c>
+      <c r="K38"/>
+      <c r="L38" s="11">
+        <f t="shared" si="2"/>
+        <v>2473</v>
+      </c>
+      <c r="M38" s="13">
+        <f t="shared" si="3"/>
+        <v>2.3039370959026639E-2</v>
+      </c>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+      <c r="X38"/>
+      <c r="Y38"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
+        <v>907</v>
+      </c>
+      <c r="B39" s="9">
+        <v>69053</v>
+      </c>
+      <c r="C39" s="9">
+        <v>82618</v>
+      </c>
+      <c r="D39" s="9">
+        <v>50574</v>
+      </c>
+      <c r="E39" s="9">
+        <v>65121</v>
+      </c>
+      <c r="F39" s="9">
+        <v>75265</v>
+      </c>
+      <c r="G39" s="9">
+        <v>82631</v>
+      </c>
+      <c r="H39"/>
+      <c r="I39" s="11">
+        <f t="shared" si="0"/>
+        <v>6212</v>
+      </c>
+      <c r="J39" s="13">
+        <f t="shared" si="1"/>
+        <v>8.9959885884755231E-2</v>
+      </c>
+      <c r="K39"/>
+      <c r="L39" s="11">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="M39" s="13">
+        <f t="shared" si="3"/>
+        <v>1.5735069839495353E-4</v>
+      </c>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+      <c r="S39"/>
+      <c r="T39"/>
+      <c r="U39"/>
+      <c r="V39"/>
+      <c r="W39"/>
+      <c r="X39"/>
+      <c r="Y39"/>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
+        <v>923</v>
+      </c>
+      <c r="B40" s="9">
+        <v>822060</v>
+      </c>
+      <c r="C40" s="9">
+        <v>940140</v>
+      </c>
+      <c r="D40" s="9">
+        <v>587002</v>
+      </c>
+      <c r="E40" s="9">
+        <v>706563</v>
+      </c>
+      <c r="F40" s="9">
+        <v>855266</v>
+      </c>
+      <c r="G40" s="9">
+        <v>965282</v>
+      </c>
+      <c r="H40"/>
+      <c r="I40" s="11">
+        <f t="shared" si="0"/>
+        <v>33206</v>
+      </c>
+      <c r="J40" s="13">
+        <f t="shared" si="1"/>
+        <v>4.0393645232708053E-2</v>
+      </c>
+      <c r="K40"/>
+      <c r="L40" s="11">
+        <f t="shared" si="2"/>
+        <v>25142</v>
+      </c>
+      <c r="M40" s="13">
+        <f t="shared" si="3"/>
+        <v>2.6742825536622217E-2</v>
+      </c>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
+      <c r="U40"/>
+      <c r="V40"/>
+      <c r="W40"/>
+      <c r="X40"/>
+      <c r="Y40"/>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A41"/>
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41"/>
+      <c r="T41"/>
+      <c r="U41"/>
+      <c r="V41"/>
+      <c r="W41"/>
+      <c r="X41"/>
+      <c r="Y41"/>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A42"/>
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42"/>
+      <c r="P42"/>
+      <c r="Q42"/>
+      <c r="R42"/>
+      <c r="S42"/>
+      <c r="T42"/>
+      <c r="U42"/>
+      <c r="V42"/>
+      <c r="W42"/>
+      <c r="X42"/>
+      <c r="Y42"/>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A43"/>
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43"/>
+      <c r="P43"/>
+      <c r="Q43"/>
+      <c r="R43"/>
+      <c r="S43"/>
+      <c r="T43"/>
+      <c r="U43"/>
+      <c r="V43"/>
+      <c r="W43"/>
+      <c r="X43"/>
+      <c r="Y43"/>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A44"/>
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
+      <c r="P44"/>
+      <c r="Q44"/>
+      <c r="R44"/>
+      <c r="S44"/>
+      <c r="T44"/>
+      <c r="U44"/>
+      <c r="V44"/>
+      <c r="W44"/>
+      <c r="X44"/>
+      <c r="Y44"/>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A45"/>
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+      <c r="S45"/>
+      <c r="T45"/>
+      <c r="U45"/>
+      <c r="V45"/>
+      <c r="W45"/>
+      <c r="X45"/>
+      <c r="Y45"/>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A46"/>
+      <c r="B46"/>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+      <c r="O46"/>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+      <c r="S46"/>
+      <c r="T46"/>
+      <c r="U46"/>
+      <c r="V46"/>
+      <c r="W46"/>
+      <c r="X46"/>
+      <c r="Y46"/>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A47"/>
+      <c r="B47"/>
+      <c r="C47"/>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+      <c r="O47"/>
+      <c r="P47"/>
+      <c r="Q47"/>
+      <c r="R47"/>
+      <c r="S47"/>
+      <c r="T47"/>
+      <c r="U47"/>
+      <c r="V47"/>
+      <c r="W47"/>
+      <c r="X47"/>
+      <c r="Y47"/>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A48"/>
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
+      <c r="O48"/>
+      <c r="P48"/>
+      <c r="Q48"/>
+      <c r="R48"/>
+      <c r="S48"/>
+      <c r="T48"/>
+      <c r="U48"/>
+      <c r="V48"/>
+      <c r="W48"/>
+      <c r="X48"/>
+      <c r="Y48"/>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A49"/>
+      <c r="B49"/>
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49"/>
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="M49"/>
+      <c r="N49"/>
+      <c r="O49"/>
+      <c r="P49"/>
+      <c r="Q49"/>
+      <c r="R49"/>
+      <c r="S49"/>
+      <c r="T49"/>
+      <c r="U49"/>
+      <c r="V49"/>
+      <c r="W49"/>
+      <c r="X49"/>
+      <c r="Y49"/>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A50"/>
+      <c r="B50"/>
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A51"/>
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A52"/>
+      <c r="B52"/>
+      <c r="C52"/>
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A53"/>
+      <c r="B53"/>
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="E53"/>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A54"/>
+      <c r="B54"/>
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="E54"/>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A55"/>
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A56"/>
+      <c r="B56"/>
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="E56"/>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A57"/>
+      <c r="B57"/>
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="E57"/>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A58"/>
+      <c r="B58"/>
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="E58"/>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A59"/>
+      <c r="B59"/>
+      <c r="C59"/>
+      <c r="D59"/>
+      <c r="E59"/>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A60"/>
+      <c r="B60"/>
+      <c r="C60"/>
+      <c r="D60"/>
+      <c r="E60"/>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A61"/>
+      <c r="B61"/>
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="E61"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
More Variance Analysis Using COUNTIFS
</commit_message>
<xml_diff>
--- a/Volume by Region Data Request v2.xlsx
+++ b/Volume by Region Data Request v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sahil\Documents\Github\excelprogress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2951E3BC-F5D7-4672-BA63-65A6AEACF1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF54BAF5-92B7-47D2-AC9F-C9048294DBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" tabRatio="458" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" tabRatio="458" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Email" sheetId="73" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3344" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3366" uniqueCount="946">
   <si>
     <t>CLID</t>
   </si>
@@ -2903,6 +2903,9 @@
   </si>
   <si>
     <t>LATAM Total</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -2914,7 +2917,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="ARIAL"/>
@@ -2935,6 +2938,12 @@
       <name val="ARIAL"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="ARIAL"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2944,11 +2953,20 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -2961,7 +2979,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -2989,9 +3007,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3004,6 +3019,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -3011,262 +3036,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Text UPPER lower" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="139">
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
+  <dxfs count="67">
     <dxf>
       <font>
         <b val="0"/>
@@ -3461,6 +3231,45 @@
     </dxf>
     <dxf>
       <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -14592,7 +14401,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F97460C6-2B1D-4429-9AE1-5403229ACA8E}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F97460C6-2B1D-4429-9AE1-5403229ACA8E}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="A51:J111" firstHeaderRow="1" firstDataRow="3" firstDataCol="2"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="descending">
@@ -15009,38 +14818,38 @@
     <dataField name="Sum of Vol" fld="2" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="12">
-    <format dxfId="73">
+    <format dxfId="41">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="74">
+    <format dxfId="40">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="75">
+    <format dxfId="39">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="76">
+    <format dxfId="38">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="77">
+    <format dxfId="37">
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="78">
+    <format dxfId="36">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="79">
+    <format dxfId="35">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="80">
+    <format dxfId="34">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="82">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="2">
@@ -15050,10 +14859,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="30">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -15210,7 +15019,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D37C5FD1-A12E-4EA3-A67C-2BFE15959C89}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D37C5FD1-A12E-4EA3-A67C-2BFE15959C89}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:E13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -15337,38 +15146,38 @@
     <dataField name="Sum of Vol" fld="2" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="12">
-    <format dxfId="126">
+    <format dxfId="53">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="125">
+    <format dxfId="52">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="124">
+    <format dxfId="51">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="123">
+    <format dxfId="50">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="122">
+    <format dxfId="49">
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="121">
+    <format dxfId="48">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="120">
+    <format dxfId="47">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="119">
+    <format dxfId="46">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="118">
+    <format dxfId="45">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="117">
+    <format dxfId="44">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="2">
@@ -15378,10 +15187,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="116">
+    <format dxfId="43">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="115">
+    <format dxfId="42">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -15538,7 +15347,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B3596AE5-7ABE-4BFD-935E-B17364891890}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B3596AE5-7ABE-4BFD-935E-B17364891890}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A33:G40" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -15660,38 +15469,38 @@
     <dataField name="Sum of Vol" fld="2" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="12">
-    <format dxfId="138">
+    <format dxfId="65">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="137">
+    <format dxfId="64">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="136">
+    <format dxfId="63">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="135">
+    <format dxfId="62">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="134">
+    <format dxfId="61">
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="133">
+    <format dxfId="60">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="132">
+    <format dxfId="59">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="131">
+    <format dxfId="58">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="130">
+    <format dxfId="57">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="129">
+    <format dxfId="56">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="2">
@@ -15701,10 +15510,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="128">
+    <format dxfId="55">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="127">
+    <format dxfId="54">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -15865,7 +15674,7 @@
   <autoFilter ref="A1:H29" xr:uid="{8B428AE4-E774-4CE8-97EC-404D39F1F4CC}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{1CDCD11C-7559-4D60-926A-FEA8FCEA1711}" name="CLID"/>
-    <tableColumn id="2" xr3:uid="{1FB599A4-0D12-43C4-95E3-48CBC7B8F1B9}" name="Date" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{1FB599A4-0D12-43C4-95E3-48CBC7B8F1B9}" name="Date" dataDxfId="66"/>
     <tableColumn id="3" xr3:uid="{BBF891A3-B9BB-4CB2-AB23-59B0152575E2}" name="Vol"/>
     <tableColumn id="4" xr3:uid="{89AEAA78-E28E-45BE-BCCA-49E576CC1B74}" name="LEN"/>
     <tableColumn id="5" xr3:uid="{9B6D4E26-0525-4A95-9621-2E256C9C3D2C}" name="Index Math Region ID"/>
@@ -15878,28 +15687,28 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{406B180F-939D-4E8E-A198-0941B7059A16}" name="VolumebyClient" displayName="VolumebyClient" ref="A1:H908" totalsRowShown="0" headerRowDxfId="114">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{406B180F-939D-4E8E-A198-0941B7059A16}" name="VolumebyClient" displayName="VolumebyClient" ref="A1:H908" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="A1:H908" xr:uid="{406B180F-939D-4E8E-A198-0941B7059A16}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H908">
     <sortCondition ref="G2:G908"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{281B7314-368E-437E-A5A8-DADE21D6AED8}" name="CLID" dataDxfId="113"/>
-    <tableColumn id="2" xr3:uid="{62D985AE-158F-47B9-BB68-6B22B444CD12}" name="Date" dataDxfId="112"/>
-    <tableColumn id="3" xr3:uid="{3869AADC-2963-49C7-A2A6-AF867F0A8C66}" name="Vol" dataDxfId="111" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{3216742F-1153-4858-8E14-8A2A7D1785F7}" name="LEN" dataDxfId="110">
+    <tableColumn id="1" xr3:uid="{281B7314-368E-437E-A5A8-DADE21D6AED8}" name="CLID" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{62D985AE-158F-47B9-BB68-6B22B444CD12}" name="Date" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{3869AADC-2963-49C7-A2A6-AF867F0A8C66}" name="Vol" dataDxfId="26" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{3216742F-1153-4858-8E14-8A2A7D1785F7}" name="LEN" dataDxfId="25">
       <calculatedColumnFormula>LEN(VolumebyClient[[#This Row],[CLID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{16347095-5BED-454C-BD70-B64E9D0FB879}" name="Index Math Region ID" dataDxfId="109">
+    <tableColumn id="6" xr3:uid="{16347095-5BED-454C-BD70-B64E9D0FB879}" name="Index Math Region ID" dataDxfId="24">
       <calculatedColumnFormula>INDEX(GeobyClient[GEOID],MATCH(VolumebyClient[[#This Row],[CLID]],GeobyClient[Right],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1DE9ED6D-1605-4183-A5E0-1D444447B5BF}" name="Region Name" dataDxfId="108">
+    <tableColumn id="5" xr3:uid="{1DE9ED6D-1605-4183-A5E0-1D444447B5BF}" name="Region Name" dataDxfId="23">
       <calculatedColumnFormula>VLOOKUP(VolumebyClient[[#This Row],[Index Math Region ID]],GEONames[[GEOID]:[GEO Name]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E9252E94-A500-4F10-8FC7-6B5270C5364E}" name="Quarter" dataDxfId="107">
+    <tableColumn id="7" xr3:uid="{E9252E94-A500-4F10-8FC7-6B5270C5364E}" name="Quarter" dataDxfId="22">
       <calculatedColumnFormula>"Q"&amp;ROUNDUP(MONTH(VolumebyClient[[#This Row],[Date]])/3,0) &amp;" "&amp; YEAR(VolumebyClient[[#This Row],[Date]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C2F6A2AF-9354-4D01-B19A-356D53214F43}" name="Quarter by Vlookup" dataDxfId="106">
+    <tableColumn id="8" xr3:uid="{C2F6A2AF-9354-4D01-B19A-356D53214F43}" name="Quarter by Vlookup" dataDxfId="21">
       <calculatedColumnFormula>VLOOKUP(VolumebyClient[[#This Row],[Date]],Quarters[],3,TRUE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -15908,37 +15717,37 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{14F98703-7709-4799-96B7-DEF2AB592176}" name="Quarters" displayName="Quarters" ref="P1:R7" totalsRowShown="0" headerRowDxfId="105">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{14F98703-7709-4799-96B7-DEF2AB592176}" name="Quarters" displayName="Quarters" ref="P1:R7" totalsRowShown="0" headerRowDxfId="20">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0CBD38A7-5922-499C-B3C6-C1D4D12C14A8}" name="Date Start" dataDxfId="104">
+    <tableColumn id="1" xr3:uid="{0CBD38A7-5922-499C-B3C6-C1D4D12C14A8}" name="Date Start" dataDxfId="19">
       <calculatedColumnFormula>Q1+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{573B04AF-E405-4F8C-A914-DBE0D184EC9D}" name="Date End" dataDxfId="103"/>
-    <tableColumn id="3" xr3:uid="{512171E3-0CEE-4260-902B-9B707E0FA464}" name="Name" dataDxfId="102"/>
+    <tableColumn id="2" xr3:uid="{573B04AF-E405-4F8C-A914-DBE0D184EC9D}" name="Date End" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{512171E3-0CEE-4260-902B-9B707E0FA464}" name="Name" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E311F35B-2E55-4952-8583-E766E50A2002}" name="GeobyClient" displayName="GeobyClient" ref="A1:G54" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E311F35B-2E55-4952-8583-E766E50A2002}" name="GeobyClient" displayName="GeobyClient" ref="A1:G54" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:G54" xr:uid="{E311F35B-2E55-4952-8583-E766E50A2002}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{08395CE6-5435-4D79-9F33-4BAF0034A67C}" name="CLID" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{A4CD2883-44A3-490F-9756-2CD00F301255}" name="GEOID" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{1912F280-065B-4FA3-B6C0-FD1AC2786982}" name="LEN" dataDxfId="97">
+    <tableColumn id="1" xr3:uid="{08395CE6-5435-4D79-9F33-4BAF0034A67C}" name="CLID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{A4CD2883-44A3-490F-9756-2CD00F301255}" name="GEOID" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{1912F280-065B-4FA3-B6C0-FD1AC2786982}" name="LEN" dataDxfId="12">
       <calculatedColumnFormula>LEN(GeobyClient[[#This Row],[CLID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0E588837-968D-4D43-B878-D29468BBA5E8}" name="Mid" dataDxfId="96">
+    <tableColumn id="4" xr3:uid="{0E588837-968D-4D43-B878-D29468BBA5E8}" name="Mid" dataDxfId="11">
       <calculatedColumnFormula>MID(GeobyClient[[#This Row],[CLID]],3,7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{88E87899-63AD-4FDE-8A1A-B2DC526B95AB}" name="Right" dataDxfId="95">
+    <tableColumn id="5" xr3:uid="{88E87899-63AD-4FDE-8A1A-B2DC526B95AB}" name="Right" dataDxfId="10">
       <calculatedColumnFormula>RIGHT(GeobyClient[[#This Row],[CLID]],7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{FCF3FA03-E7C7-481E-9D09-023637C4C393}" name="Test" dataDxfId="94">
+    <tableColumn id="6" xr3:uid="{FCF3FA03-E7C7-481E-9D09-023637C4C393}" name="Test" dataDxfId="9">
       <calculatedColumnFormula>GeobyClient[[#This Row],[Right]]=GeobyClient[[#This Row],[Mid]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{48FEDD23-08C0-4676-AB94-87F464ABE65C}" name="Region" dataDxfId="93">
+    <tableColumn id="7" xr3:uid="{48FEDD23-08C0-4676-AB94-87F464ABE65C}" name="Region" dataDxfId="8">
       <calculatedColumnFormula>VLOOKUP(GeobyClient[[#This Row],[GEOID]],GEONames[[GEOID]:[GEO Name]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -15947,12 +15756,12 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{73CE4639-4172-46C1-8556-28321ADFD967}" name="GEONames" displayName="GEONames" ref="J1:L6" totalsRowCount="1" headerRowDxfId="92" dataDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{73CE4639-4172-46C1-8556-28321ADFD967}" name="GEONames" displayName="GEONames" ref="J1:L6" totalsRowCount="1" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="J1:L5" xr:uid="{73CE4639-4172-46C1-8556-28321ADFD967}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A06CC5BB-9608-4621-894C-728B35C38EB5}" name="GEOID" dataDxfId="90" totalsRowDxfId="89"/>
-    <tableColumn id="2" xr3:uid="{C85A19C8-B7B0-4EC8-90DF-70D56F599F3A}" name="GEO Name" dataDxfId="88" totalsRowDxfId="87"/>
-    <tableColumn id="3" xr3:uid="{FC923D28-8982-4073-94D2-0E68AD4DFB30}" name="Volume" totalsRowFunction="sum" dataDxfId="86" totalsRowDxfId="85" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="1" xr3:uid="{A06CC5BB-9608-4621-894C-728B35C38EB5}" name="GEOID" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{C85A19C8-B7B0-4EC8-90DF-70D56F599F3A}" name="GEO Name" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{FC923D28-8982-4073-94D2-0E68AD4DFB30}" name="Volume" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>SUMIFS(VolumebyClient[Vol],VolumebyClient[Index Math Region ID],GEONames[[#This Row],[GEOID]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -16290,150 +16099,150 @@
   <sheetFormatPr defaultRowHeight="13.15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>897</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
     </row>
     <row r="5" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
     </row>
     <row r="6" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
     </row>
     <row r="7" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
     </row>
     <row r="10" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
     </row>
     <row r="12" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
     </row>
     <row r="13" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
     </row>
     <row r="14" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
     </row>
     <row r="15" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
     </row>
     <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -25523,10 +25332,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472D7B1D-3022-458C-99D2-1C6B8FA100F0}">
-  <dimension ref="A3:Y111"/>
+  <dimension ref="A3:Y129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G19" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25976,7 +25785,7 @@
         <v>934</v>
       </c>
       <c r="N35"/>
-      <c r="O35" s="17" t="s">
+      <c r="O35" s="16" t="s">
         <v>936</v>
       </c>
       <c r="P35"/>
@@ -26031,19 +25840,19 @@
         <v>3.4483835051975387E-2</v>
       </c>
       <c r="N36"/>
-      <c r="O36" s="14">
+      <c r="O36" s="13">
         <f>C36/(1-J36)</f>
         <v>600918.05953123746</v>
       </c>
-      <c r="P36" s="15">
+      <c r="P36" s="14">
         <f>O36/$O$40</f>
         <v>0.61336055121642019</v>
       </c>
-      <c r="Q36" s="14">
+      <c r="Q36" s="13">
         <f>O36-G36</f>
         <v>4416.0595312374644</v>
       </c>
-      <c r="R36" s="16">
+      <c r="R36" s="15">
         <f>Q36/$Q$40</f>
         <v>0.30598596603620037</v>
       </c>
@@ -26095,19 +25904,19 @@
         <v>1.5970869870827187E-2</v>
       </c>
       <c r="N37"/>
-      <c r="O37" s="14">
+      <c r="O37" s="13">
         <f t="shared" ref="O37:O40" si="4">C37/(1-J37)</f>
         <v>176371.68544329898</v>
       </c>
-      <c r="P37" s="15">
+      <c r="P37" s="14">
         <f>O37/$O$40</f>
         <v>0.18002360302976958</v>
       </c>
-      <c r="Q37" s="14">
+      <c r="Q37" s="13">
         <f>O37-G37</f>
         <v>33.685443298978498</v>
       </c>
-      <c r="R37" s="15">
+      <c r="R37" s="14">
         <f>Q37/$Q$40</f>
         <v>2.334043016468868E-3</v>
       </c>
@@ -26159,19 +25968,19 @@
         <v>2.3039370959026639E-2</v>
       </c>
       <c r="N38"/>
-      <c r="O38" s="14">
+      <c r="O38" s="13">
         <f t="shared" si="4"/>
         <v>112069.60944009421</v>
       </c>
-      <c r="P38" s="15">
+      <c r="P38" s="14">
         <f>O38/$O$40</f>
         <v>0.11439010083073041</v>
       </c>
-      <c r="Q38" s="14">
+      <c r="Q38" s="13">
         <f>O38-G38</f>
         <v>2258.6094400942093</v>
       </c>
-      <c r="R38" s="15">
+      <c r="R38" s="14">
         <f>Q38/$Q$40</f>
         <v>0.15649761660528339</v>
       </c>
@@ -26223,19 +26032,19 @@
         <v>1.5735069839495353E-4</v>
       </c>
       <c r="N39"/>
-      <c r="O39" s="14">
+      <c r="O39" s="13">
         <f t="shared" si="4"/>
         <v>90785.009054598122</v>
       </c>
-      <c r="P39" s="15">
+      <c r="P39" s="14">
         <f>O39/$O$40</f>
         <v>9.2664785677025227E-2</v>
       </c>
-      <c r="Q39" s="14">
+      <c r="Q39" s="13">
         <f>O39-G39</f>
         <v>8154.009054598122</v>
       </c>
-      <c r="R39" s="15">
+      <c r="R39" s="14">
         <f>Q39/$Q$40</f>
         <v>0.56498611941039234</v>
       </c>
@@ -26287,19 +26096,19 @@
         <v>2.6742825536622217E-2</v>
       </c>
       <c r="N40"/>
-      <c r="O40" s="14">
+      <c r="O40" s="13">
         <f t="shared" si="4"/>
         <v>979714.22899547953</v>
       </c>
-      <c r="P40" s="15">
+      <c r="P40" s="14">
         <f>O40/$O$40</f>
         <v>1</v>
       </c>
-      <c r="Q40" s="14">
+      <c r="Q40" s="13">
         <f>O40-G40</f>
         <v>14432.228995479527</v>
       </c>
-      <c r="R40" s="15">
+      <c r="R40" s="14">
         <f>Q40/$Q$40</f>
         <v>1</v>
       </c>
@@ -28444,6 +28253,379 @@
       </c>
       <c r="J111" s="9">
         <v>1820548</v>
+      </c>
+    </row>
+    <row r="115" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C115" s="19" t="s">
+        <v>925</v>
+      </c>
+      <c r="D115" s="19" t="s">
+        <v>925</v>
+      </c>
+      <c r="E115" s="19" t="s">
+        <v>925</v>
+      </c>
+      <c r="F115" s="19" t="s">
+        <v>925</v>
+      </c>
+      <c r="G115" s="19"/>
+      <c r="H115" s="19" t="s">
+        <v>926</v>
+      </c>
+      <c r="I115" s="19" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="116" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C116" s="19" t="s">
+        <v>927</v>
+      </c>
+      <c r="D116" s="19" t="s">
+        <v>928</v>
+      </c>
+      <c r="E116" s="19" t="s">
+        <v>929</v>
+      </c>
+      <c r="F116" s="19" t="s">
+        <v>930</v>
+      </c>
+      <c r="G116" s="19"/>
+      <c r="H116" s="19" t="s">
+        <v>927</v>
+      </c>
+      <c r="I116" s="19" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="117" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B117" s="21" t="s">
+        <v>898</v>
+      </c>
+      <c r="C117" s="3">
+        <f>COUNTIFS(C$54:C$109,"&gt;0",$A$54:$A$109,$B117)</f>
+        <v>18</v>
+      </c>
+      <c r="D117" s="3">
+        <f t="shared" ref="D117:F120" si="5">COUNTIFS(D$54:D$109,"&gt;0",$A$54:$A$109,$B117)</f>
+        <v>19</v>
+      </c>
+      <c r="E117" s="3">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="F117" s="3">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="H117" s="3">
+        <f>COUNTIFS(H$54:H$109,"&gt;0",$A$54:$A$109,$B117)</f>
+        <v>20</v>
+      </c>
+      <c r="I117" s="3">
+        <f>COUNTIFS(I$54:I$109,"&gt;0",$A$54:$A$109,$B117)</f>
+        <v>20</v>
+      </c>
+      <c r="K117" s="3">
+        <f>I117-D117</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B118" s="21" t="s">
+        <v>899</v>
+      </c>
+      <c r="C118" s="3">
+        <f t="shared" ref="C118:C120" si="6">COUNTIFS(C$54:C$109,"&gt;0",$A$54:$A$109,$B118)</f>
+        <v>8</v>
+      </c>
+      <c r="D118" s="3">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="E118" s="3">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="F118" s="3">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="H118" s="3">
+        <f>COUNTIFS(H$54:H$109,"&gt;0",$A$54:$A$109,$B118)</f>
+        <v>8</v>
+      </c>
+      <c r="I118" s="3">
+        <f>COUNTIFS(I$54:I$109,"&gt;0",$A$54:$A$109,$B118)</f>
+        <v>8</v>
+      </c>
+      <c r="K118" s="3">
+        <f t="shared" ref="K118:K121" si="7">I118-D118</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B119" s="21" t="s">
+        <v>908</v>
+      </c>
+      <c r="C119" s="3">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="D119" s="3">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="E119" s="3">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="F119" s="3">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="H119" s="3">
+        <f>COUNTIFS(H$54:H$109,"&gt;0",$A$54:$A$109,$B119)</f>
+        <v>14</v>
+      </c>
+      <c r="I119" s="3">
+        <f>COUNTIFS(I$54:I$109,"&gt;0",$A$54:$A$109,$B119)</f>
+        <v>13</v>
+      </c>
+      <c r="K119" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B120" s="21" t="s">
+        <v>907</v>
+      </c>
+      <c r="C120" s="3">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="D120" s="3">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E120" s="3">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="F120" s="3">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="H120" s="3">
+        <f>COUNTIFS(H$54:H$109,"&gt;0",$A$54:$A$109,$B120)</f>
+        <v>11</v>
+      </c>
+      <c r="I120" s="3">
+        <f>COUNTIFS(I$54:I$109,"&gt;0",$A$54:$A$109,$B120)</f>
+        <v>9</v>
+      </c>
+      <c r="K120" s="3">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="121" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B121" s="20" t="s">
+        <v>945</v>
+      </c>
+      <c r="C121" s="20">
+        <f>SUM(C117:C120)</f>
+        <v>49</v>
+      </c>
+      <c r="D121" s="20">
+        <f t="shared" ref="D121:I121" si="8">SUM(D117:D120)</f>
+        <v>50</v>
+      </c>
+      <c r="E121" s="20">
+        <f t="shared" si="8"/>
+        <v>52</v>
+      </c>
+      <c r="F121" s="20">
+        <f t="shared" si="8"/>
+        <v>53</v>
+      </c>
+      <c r="G121" s="18"/>
+      <c r="H121" s="20">
+        <f t="shared" si="8"/>
+        <v>53</v>
+      </c>
+      <c r="I121" s="20">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="K121" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B125" s="21" t="s">
+        <v>898</v>
+      </c>
+      <c r="C125" s="5">
+        <f>B36/C117</f>
+        <v>28301.055555555555</v>
+      </c>
+      <c r="D125" s="5">
+        <f t="shared" ref="D125:F125" si="9">C36/D117</f>
+        <v>30348.315789473683</v>
+      </c>
+      <c r="E125" s="5">
+        <f t="shared" si="9"/>
+        <v>19141.78947368421</v>
+      </c>
+      <c r="F125" s="5">
+        <f t="shared" si="9"/>
+        <v>21601.7</v>
+      </c>
+      <c r="H125" s="5">
+        <f>F36/H117</f>
+        <v>26500.95</v>
+      </c>
+      <c r="I125" s="5">
+        <f>G36/I117</f>
+        <v>29825.1</v>
+      </c>
+      <c r="K125" s="22">
+        <f>I125/D125-1</f>
+        <v>-1.7240356700623294E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B126" s="21" t="s">
+        <v>899</v>
+      </c>
+      <c r="C126" s="5">
+        <f t="shared" ref="C126:F126" si="10">B37/C118</f>
+        <v>18481.5</v>
+      </c>
+      <c r="D126" s="5">
+        <f t="shared" si="10"/>
+        <v>21695.75</v>
+      </c>
+      <c r="E126" s="5">
+        <f t="shared" si="10"/>
+        <v>12942</v>
+      </c>
+      <c r="F126" s="5">
+        <f t="shared" si="10"/>
+        <v>16158</v>
+      </c>
+      <c r="H126" s="5">
+        <f>F37/H118</f>
+        <v>18775.5</v>
+      </c>
+      <c r="I126" s="5">
+        <f>G37/I118</f>
+        <v>22042.25</v>
+      </c>
+      <c r="K126" s="22">
+        <f t="shared" ref="K126:K129" si="11">I126/D126-1</f>
+        <v>1.5970869870827187E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B127" s="21" t="s">
+        <v>908</v>
+      </c>
+      <c r="C127" s="5">
+        <f t="shared" ref="C127:F127" si="12">B38/C119</f>
+        <v>7364.3076923076924</v>
+      </c>
+      <c r="D127" s="5">
+        <f t="shared" si="12"/>
+        <v>8256.7692307692305</v>
+      </c>
+      <c r="E127" s="5">
+        <f t="shared" si="12"/>
+        <v>4942.7142857142853</v>
+      </c>
+      <c r="F127" s="5">
+        <f t="shared" si="12"/>
+        <v>5724.5714285714284</v>
+      </c>
+      <c r="H127" s="5">
+        <f>F38/H119</f>
+        <v>7127</v>
+      </c>
+      <c r="I127" s="5">
+        <f>G38/I119</f>
+        <v>8447</v>
+      </c>
+      <c r="K127" s="22">
+        <f t="shared" si="11"/>
+        <v>2.3039370959026639E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B128" s="21" t="s">
+        <v>907</v>
+      </c>
+      <c r="C128" s="5">
+        <f t="shared" ref="C128:F129" si="13">B39/C120</f>
+        <v>6905.3</v>
+      </c>
+      <c r="D128" s="5">
+        <f t="shared" si="13"/>
+        <v>8261.7999999999993</v>
+      </c>
+      <c r="E128" s="5">
+        <f t="shared" si="13"/>
+        <v>4597.636363636364</v>
+      </c>
+      <c r="F128" s="5">
+        <f t="shared" si="13"/>
+        <v>5920.090909090909</v>
+      </c>
+      <c r="H128" s="5">
+        <f>F39/H120</f>
+        <v>6842.272727272727</v>
+      </c>
+      <c r="I128" s="5">
+        <f>G39/I120</f>
+        <v>9181.2222222222226</v>
+      </c>
+      <c r="K128" s="22">
+        <f t="shared" si="11"/>
+        <v>0.11128594522043911</v>
+      </c>
+    </row>
+    <row r="129" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B129" s="20" t="s">
+        <v>945</v>
+      </c>
+      <c r="C129" s="5">
+        <f>B40/C121</f>
+        <v>16776.734693877552</v>
+      </c>
+      <c r="D129" s="5">
+        <f t="shared" si="13"/>
+        <v>18802.8</v>
+      </c>
+      <c r="E129" s="5">
+        <f t="shared" si="13"/>
+        <v>11288.5</v>
+      </c>
+      <c r="F129" s="5">
+        <f t="shared" si="13"/>
+        <v>13331.377358490567</v>
+      </c>
+      <c r="H129" s="5">
+        <f>F40/H121</f>
+        <v>16137.094339622641</v>
+      </c>
+      <c r="I129" s="5">
+        <f>G40/I121</f>
+        <v>19305.64</v>
+      </c>
+      <c r="K129" s="22">
+        <f t="shared" si="11"/>
+        <v>2.6742825536622217E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Brief Analysis And Pressure Testing Conclusion
</commit_message>
<xml_diff>
--- a/Volume by Region Data Request v2.xlsx
+++ b/Volume by Region Data Request v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sahil\Documents\Github\excelprogress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF54BAF5-92B7-47D2-AC9F-C9048294DBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455257AF-4BE9-41FA-9352-B01571073CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" tabRatio="458" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3366" uniqueCount="946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3375" uniqueCount="950">
   <si>
     <t>CLID</t>
   </si>
@@ -2906,6 +2906,18 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>2 customers left region in Q2, taking 7k in volume away</t>
+  </si>
+  <si>
+    <t>Q2 YOY growth slowed from Q1 growth of 4% down to 2.7% primarily driven by:</t>
+  </si>
+  <si>
+    <t>-.7% or 7k volume decline from loss of two customers in LATAM driving overall growth for region down from 9% in Q1 to flat in Q2 YOY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">same store sales slower than expected in Q2 vs Q1 in YOY, comprising of majority of remaining variance </t>
   </si>
 </sst>
 </file>
@@ -2979,7 +2991,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -3019,9 +3031,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -3029,6 +3038,10 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -16099,150 +16112,150 @@
   <sheetFormatPr defaultRowHeight="13.15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="22" t="s">
         <v>897</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
     </row>
     <row r="7" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
     </row>
     <row r="8" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
     </row>
     <row r="9" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
     </row>
     <row r="12" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
     </row>
     <row r="14" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
     </row>
     <row r="15" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
     </row>
     <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -25332,10 +25345,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472D7B1D-3022-458C-99D2-1C6B8FA100F0}">
-  <dimension ref="A3:Y129"/>
+  <dimension ref="A3:Y136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="O78" sqref="O78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26048,6 +26061,9 @@
         <f>Q39/$Q$40</f>
         <v>0.56498611941039234</v>
       </c>
+      <c r="S39" s="3" t="s">
+        <v>946</v>
+      </c>
       <c r="T39"/>
       <c r="U39"/>
       <c r="V39"/>
@@ -26138,7 +26154,9 @@
       <c r="P41"/>
       <c r="Q41"/>
       <c r="R41"/>
-      <c r="S41"/>
+      <c r="S41" s="3" t="s">
+        <v>947</v>
+      </c>
       <c r="T41"/>
       <c r="U41"/>
       <c r="V41"/>
@@ -26165,7 +26183,9 @@
       <c r="P42"/>
       <c r="Q42"/>
       <c r="R42"/>
-      <c r="S42"/>
+      <c r="S42" s="23" t="s">
+        <v>948</v>
+      </c>
       <c r="T42"/>
       <c r="U42"/>
       <c r="V42"/>
@@ -26192,7 +26212,9 @@
       <c r="P43"/>
       <c r="Q43"/>
       <c r="R43"/>
-      <c r="S43"/>
+      <c r="S43" s="3" t="s">
+        <v>949</v>
+      </c>
       <c r="T43"/>
       <c r="U43"/>
       <c r="V43"/>
@@ -26467,6 +26489,10 @@
       <c r="J54" s="9">
         <v>203625</v>
       </c>
+      <c r="L54" s="3">
+        <f>I54/D54-1</f>
+        <v>3.2046377493967437E-2</v>
+      </c>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
@@ -26499,6 +26525,10 @@
       <c r="J55" s="9">
         <v>184133</v>
       </c>
+      <c r="L55" s="3">
+        <f t="shared" ref="L55:L56" si="5">I55/D55-1</f>
+        <v>1.5301154541660811E-2</v>
+      </c>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
@@ -26531,6 +26561,10 @@
       <c r="J56" s="9">
         <v>151600</v>
       </c>
+      <c r="L56" s="3">
+        <f t="shared" si="5"/>
+        <v>3.5687619433300899E-2</v>
+      </c>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
@@ -26788,7 +26822,7 @@
         <v>10704</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>898</v>
       </c>
@@ -26820,7 +26854,7 @@
         <v>10471</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>898</v>
       </c>
@@ -26852,7 +26886,7 @@
         <v>10214</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>898</v>
       </c>
@@ -26884,7 +26918,7 @@
         <v>8199</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>898</v>
       </c>
@@ -26914,7 +26948,7 @@
         <v>11348</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>898</v>
       </c>
@@ -26946,7 +26980,7 @@
         <v>7356</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>898</v>
       </c>
@@ -26978,7 +27012,7 @@
         <v>5373</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>898</v>
       </c>
@@ -27010,7 +27044,7 @@
         <v>5611</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>898</v>
       </c>
@@ -27042,7 +27076,7 @@
         <v>4125</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>898</v>
       </c>
@@ -27068,7 +27102,7 @@
         <v>7786</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>941</v>
       </c>
@@ -27097,7 +27131,7 @@
         <v>1126521</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>899</v>
       </c>
@@ -27128,8 +27162,12 @@
       <c r="J75" s="9">
         <v>166431</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L75" s="3">
+        <f>I75/D75-1</f>
+        <v>1.3716013418079154E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>899</v>
       </c>
@@ -27160,8 +27198,12 @@
       <c r="J76" s="9">
         <v>134788</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L76" s="3">
+        <f t="shared" ref="L76:L78" si="6">I76/D76-1</f>
+        <v>2.9999131718329464E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>899</v>
       </c>
@@ -27192,8 +27234,12 @@
       <c r="J77" s="9">
         <v>7033</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L77" s="3">
+        <f t="shared" si="6"/>
+        <v>-5.3475935828872778E-4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>899</v>
       </c>
@@ -27225,7 +27271,7 @@
         <v>6808</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>899</v>
       </c>
@@ -27257,7 +27303,7 @@
         <v>3729</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>899</v>
       </c>
@@ -27289,7 +27335,7 @@
         <v>3834</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>899</v>
       </c>
@@ -27321,7 +27367,7 @@
         <v>3309</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>899</v>
       </c>
@@ -27353,7 +27399,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>942</v>
       </c>
@@ -27382,7 +27428,7 @@
         <v>326542</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>908</v>
       </c>
@@ -27413,8 +27459,12 @@
       <c r="J84" s="9">
         <v>101005</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L84" s="3">
+        <f>I84/D84-1</f>
+        <v>9.1865011578027289E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>908</v>
       </c>
@@ -27445,8 +27495,12 @@
       <c r="J85" s="9">
         <v>58148</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L85" s="3">
+        <f t="shared" ref="L85:L87" si="7">I85/D85-1</f>
+        <v>2.2120414373141051E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>908</v>
       </c>
@@ -27477,8 +27531,12 @@
       <c r="J86" s="9">
         <v>9602</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L86" s="3">
+        <f t="shared" si="7"/>
+        <v>3.4714003944773086E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>908</v>
       </c>
@@ -27509,8 +27567,12 @@
       <c r="J87" s="9">
         <v>8593</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L87" s="3">
+        <f t="shared" si="7"/>
+        <v>1.6408181613845718E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>908</v>
       </c>
@@ -27542,7 +27604,7 @@
         <v>6564</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>908</v>
       </c>
@@ -27574,7 +27636,7 @@
         <v>6256</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>908</v>
       </c>
@@ -27606,7 +27668,7 @@
         <v>5372</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>908</v>
       </c>
@@ -27638,7 +27700,7 @@
         <v>5123</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>908</v>
       </c>
@@ -27670,7 +27732,7 @@
         <v>2652</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>908</v>
       </c>
@@ -27702,7 +27764,7 @@
         <v>1792</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>908</v>
       </c>
@@ -27730,7 +27792,7 @@
         <v>2386</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>908</v>
       </c>
@@ -27762,7 +27824,7 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>908</v>
       </c>
@@ -27792,7 +27854,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>908</v>
       </c>
@@ -27824,7 +27886,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>943</v>
       </c>
@@ -27853,7 +27915,7 @@
         <v>209589</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>907</v>
       </c>
@@ -27884,8 +27946,12 @@
       <c r="J99" s="9">
         <v>92414</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L99" s="3">
+        <f>I99/D99-1</f>
+        <v>2.7674186382996124E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>907</v>
       </c>
@@ -27916,8 +27982,12 @@
       <c r="J100" s="9">
         <v>25118</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L100" s="3">
+        <f t="shared" ref="L100:L102" si="8">I100/D100-1</f>
+        <v>2.6335761991499673E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>907</v>
       </c>
@@ -27948,8 +28018,12 @@
       <c r="J101" s="9">
         <v>9229</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L101" s="3">
+        <f t="shared" si="8"/>
+        <v>1.0386965376782076E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>907</v>
       </c>
@@ -27980,8 +28054,12 @@
       <c r="J102" s="9">
         <v>8900</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L102" s="3">
+        <f t="shared" si="8"/>
+        <v>-4.2735042735042583E-4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>907</v>
       </c>
@@ -28013,7 +28091,7 @@
         <v>5915</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>907</v>
       </c>
@@ -28045,7 +28123,7 @@
         <v>4768</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>907</v>
       </c>
@@ -28071,7 +28149,7 @@
         <v>4809</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>907</v>
       </c>
@@ -28103,7 +28181,7 @@
         <v>2972</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>907</v>
       </c>
@@ -28133,7 +28211,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>907</v>
       </c>
@@ -28165,7 +28243,7 @@
         <v>2084</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>907</v>
       </c>
@@ -28197,7 +28275,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>944</v>
       </c>
@@ -28226,7 +28304,7 @@
         <v>157896</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>923</v>
       </c>
@@ -28256,49 +28334,49 @@
       </c>
     </row>
     <row r="115" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C115" s="19" t="s">
+      <c r="C115" s="18" t="s">
         <v>925</v>
       </c>
-      <c r="D115" s="19" t="s">
+      <c r="D115" s="18" t="s">
         <v>925</v>
       </c>
-      <c r="E115" s="19" t="s">
+      <c r="E115" s="18" t="s">
         <v>925</v>
       </c>
-      <c r="F115" s="19" t="s">
+      <c r="F115" s="18" t="s">
         <v>925</v>
       </c>
-      <c r="G115" s="19"/>
-      <c r="H115" s="19" t="s">
+      <c r="G115" s="18"/>
+      <c r="H115" s="18" t="s">
         <v>926</v>
       </c>
-      <c r="I115" s="19" t="s">
+      <c r="I115" s="18" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="116" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C116" s="19" t="s">
+      <c r="C116" s="18" t="s">
         <v>927</v>
       </c>
-      <c r="D116" s="19" t="s">
+      <c r="D116" s="18" t="s">
         <v>928</v>
       </c>
-      <c r="E116" s="19" t="s">
+      <c r="E116" s="18" t="s">
         <v>929</v>
       </c>
-      <c r="F116" s="19" t="s">
+      <c r="F116" s="18" t="s">
         <v>930</v>
       </c>
-      <c r="G116" s="19"/>
-      <c r="H116" s="19" t="s">
+      <c r="G116" s="18"/>
+      <c r="H116" s="18" t="s">
         <v>927</v>
       </c>
-      <c r="I116" s="19" t="s">
+      <c r="I116" s="18" t="s">
         <v>928</v>
       </c>
     </row>
     <row r="117" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B117" s="21" t="s">
+      <c r="B117" s="20" t="s">
         <v>898</v>
       </c>
       <c r="C117" s="3">
@@ -28306,23 +28384,23 @@
         <v>18</v>
       </c>
       <c r="D117" s="3">
-        <f t="shared" ref="D117:F120" si="5">COUNTIFS(D$54:D$109,"&gt;0",$A$54:$A$109,$B117)</f>
+        <f t="shared" ref="D117:F120" si="9">COUNTIFS(D$54:D$109,"&gt;0",$A$54:$A$109,$B117)</f>
         <v>19</v>
       </c>
       <c r="E117" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
       <c r="F117" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="H117" s="3">
-        <f>COUNTIFS(H$54:H$109,"&gt;0",$A$54:$A$109,$B117)</f>
+        <f t="shared" ref="H117:I120" si="10">COUNTIFS(H$54:H$109,"&gt;0",$A$54:$A$109,$B117)</f>
         <v>20</v>
       </c>
       <c r="I117" s="3">
-        <f>COUNTIFS(I$54:I$109,"&gt;0",$A$54:$A$109,$B117)</f>
+        <f t="shared" si="10"/>
         <v>20</v>
       </c>
       <c r="K117" s="3">
@@ -28331,140 +28409,140 @@
       </c>
     </row>
     <row r="118" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B118" s="21" t="s">
+      <c r="B118" s="20" t="s">
         <v>899</v>
       </c>
       <c r="C118" s="3">
-        <f t="shared" ref="C118:C120" si="6">COUNTIFS(C$54:C$109,"&gt;0",$A$54:$A$109,$B118)</f>
+        <f t="shared" ref="C118:C120" si="11">COUNTIFS(C$54:C$109,"&gt;0",$A$54:$A$109,$B118)</f>
         <v>8</v>
       </c>
       <c r="D118" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="E118" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="F118" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="H118" s="3">
-        <f>COUNTIFS(H$54:H$109,"&gt;0",$A$54:$A$109,$B118)</f>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="I118" s="3">
-        <f>COUNTIFS(I$54:I$109,"&gt;0",$A$54:$A$109,$B118)</f>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="K118" s="3">
-        <f t="shared" ref="K118:K121" si="7">I118-D118</f>
+        <f t="shared" ref="K118:K121" si="12">I118-D118</f>
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B119" s="21" t="s">
+      <c r="B119" s="20" t="s">
         <v>908</v>
       </c>
       <c r="C119" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
       <c r="D119" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="E119" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="F119" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="H119" s="3">
-        <f>COUNTIFS(H$54:H$109,"&gt;0",$A$54:$A$109,$B119)</f>
+        <f t="shared" si="10"/>
         <v>14</v>
       </c>
       <c r="I119" s="3">
-        <f>COUNTIFS(I$54:I$109,"&gt;0",$A$54:$A$109,$B119)</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="K119" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B120" s="21" t="s">
+      <c r="B120" s="20" t="s">
         <v>907</v>
       </c>
       <c r="C120" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="D120" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="E120" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="F120" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="H120" s="3">
-        <f>COUNTIFS(H$54:H$109,"&gt;0",$A$54:$A$109,$B120)</f>
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
       <c r="I120" s="3">
-        <f>COUNTIFS(I$54:I$109,"&gt;0",$A$54:$A$109,$B120)</f>
+        <f t="shared" si="10"/>
         <v>9</v>
       </c>
       <c r="K120" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>-1</v>
       </c>
     </row>
     <row r="121" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B121" s="20" t="s">
+      <c r="B121" s="19" t="s">
         <v>945</v>
       </c>
-      <c r="C121" s="20">
+      <c r="C121" s="19">
         <f>SUM(C117:C120)</f>
         <v>49</v>
       </c>
-      <c r="D121" s="20">
-        <f t="shared" ref="D121:I121" si="8">SUM(D117:D120)</f>
+      <c r="D121" s="19">
+        <f t="shared" ref="D121:I121" si="13">SUM(D117:D120)</f>
         <v>50</v>
       </c>
-      <c r="E121" s="20">
-        <f t="shared" si="8"/>
+      <c r="E121" s="19">
+        <f t="shared" si="13"/>
         <v>52</v>
       </c>
-      <c r="F121" s="20">
-        <f t="shared" si="8"/>
+      <c r="F121" s="19">
+        <f t="shared" si="13"/>
         <v>53</v>
       </c>
-      <c r="G121" s="18"/>
-      <c r="H121" s="20">
-        <f t="shared" si="8"/>
+      <c r="G121" s="17"/>
+      <c r="H121" s="19">
+        <f t="shared" si="13"/>
         <v>53</v>
       </c>
-      <c r="I121" s="20">
-        <f t="shared" si="8"/>
+      <c r="I121" s="19">
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="K121" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B125" s="21" t="s">
+      <c r="B125" s="20" t="s">
         <v>898</v>
       </c>
       <c r="C125" s="5">
@@ -28472,131 +28550,119 @@
         <v>28301.055555555555</v>
       </c>
       <c r="D125" s="5">
-        <f t="shared" ref="D125:F125" si="9">C36/D117</f>
+        <f t="shared" ref="D125:F125" si="14">C36/D117</f>
         <v>30348.315789473683</v>
       </c>
       <c r="E125" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>19141.78947368421</v>
       </c>
       <c r="F125" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>21601.7</v>
       </c>
       <c r="H125" s="5">
-        <f>F36/H117</f>
+        <f t="shared" ref="H125:I129" si="15">F36/H117</f>
         <v>26500.95</v>
       </c>
       <c r="I125" s="5">
-        <f>G36/I117</f>
+        <f t="shared" si="15"/>
         <v>29825.1</v>
       </c>
-      <c r="K125" s="22">
-        <f>I125/D125-1</f>
-        <v>-1.7240356700623294E-2</v>
-      </c>
+      <c r="K125" s="21"/>
     </row>
     <row r="126" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B126" s="21" t="s">
+      <c r="B126" s="20" t="s">
         <v>899</v>
       </c>
       <c r="C126" s="5">
-        <f t="shared" ref="C126:F126" si="10">B37/C118</f>
+        <f t="shared" ref="C126:F126" si="16">B37/C118</f>
         <v>18481.5</v>
       </c>
       <c r="D126" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>21695.75</v>
       </c>
       <c r="E126" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>12942</v>
       </c>
       <c r="F126" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>16158</v>
       </c>
       <c r="H126" s="5">
-        <f>F37/H118</f>
+        <f t="shared" si="15"/>
         <v>18775.5</v>
       </c>
       <c r="I126" s="5">
-        <f>G37/I118</f>
+        <f t="shared" si="15"/>
         <v>22042.25</v>
       </c>
-      <c r="K126" s="22">
-        <f t="shared" ref="K126:K129" si="11">I126/D126-1</f>
-        <v>1.5970869870827187E-2</v>
-      </c>
+      <c r="K126" s="21"/>
     </row>
     <row r="127" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B127" s="21" t="s">
+      <c r="B127" s="20" t="s">
         <v>908</v>
       </c>
       <c r="C127" s="5">
-        <f t="shared" ref="C127:F127" si="12">B38/C119</f>
+        <f t="shared" ref="C127:F127" si="17">B38/C119</f>
         <v>7364.3076923076924</v>
       </c>
       <c r="D127" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>8256.7692307692305</v>
       </c>
       <c r="E127" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>4942.7142857142853</v>
       </c>
       <c r="F127" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>5724.5714285714284</v>
       </c>
       <c r="H127" s="5">
-        <f>F38/H119</f>
+        <f t="shared" si="15"/>
         <v>7127</v>
       </c>
       <c r="I127" s="5">
-        <f>G38/I119</f>
+        <f t="shared" si="15"/>
         <v>8447</v>
       </c>
-      <c r="K127" s="22">
-        <f t="shared" si="11"/>
-        <v>2.3039370959026639E-2</v>
-      </c>
+      <c r="K127" s="21"/>
     </row>
     <row r="128" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B128" s="21" t="s">
+      <c r="B128" s="20" t="s">
         <v>907</v>
       </c>
       <c r="C128" s="5">
-        <f t="shared" ref="C128:F129" si="13">B39/C120</f>
+        <f t="shared" ref="C128:F129" si="18">B39/C120</f>
         <v>6905.3</v>
       </c>
       <c r="D128" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>8261.7999999999993</v>
       </c>
       <c r="E128" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>4597.636363636364</v>
       </c>
       <c r="F128" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>5920.090909090909</v>
       </c>
       <c r="H128" s="5">
-        <f>F39/H120</f>
+        <f t="shared" si="15"/>
         <v>6842.272727272727</v>
       </c>
       <c r="I128" s="5">
-        <f>G39/I120</f>
+        <f t="shared" si="15"/>
         <v>9181.2222222222226</v>
       </c>
-      <c r="K128" s="22">
-        <f t="shared" si="11"/>
-        <v>0.11128594522043911</v>
-      </c>
+      <c r="K128" s="21"/>
     </row>
     <row r="129" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B129" s="20" t="s">
+      <c r="B129" s="19" t="s">
         <v>945</v>
       </c>
       <c r="C129" s="5">
@@ -28604,28 +28670,110 @@
         <v>16776.734693877552</v>
       </c>
       <c r="D129" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>18802.8</v>
       </c>
       <c r="E129" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>11288.5</v>
       </c>
       <c r="F129" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>13331.377358490567</v>
       </c>
       <c r="H129" s="5">
-        <f>F40/H121</f>
+        <f t="shared" si="15"/>
         <v>16137.094339622641</v>
       </c>
       <c r="I129" s="5">
-        <f>G40/I121</f>
+        <f t="shared" si="15"/>
         <v>19305.64</v>
       </c>
-      <c r="K129" s="22">
-        <f t="shared" si="11"/>
-        <v>2.6742825536622217E-2</v>
+      <c r="K129" s="21"/>
+    </row>
+    <row r="132" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B132" s="20" t="s">
+        <v>898</v>
+      </c>
+      <c r="D132" s="3">
+        <f>SUMIFS(D$54:D$109,$A$54:$A$109,$B132,$I$54:$I$109,"&gt;0")</f>
+        <v>576618</v>
+      </c>
+      <c r="I132" s="3">
+        <f>SUMIFS(I$54:I$109,$A$54:$A$109,$B132,$D$54:$D$109,"&gt;0")</f>
+        <v>592181</v>
+      </c>
+      <c r="J132" s="3">
+        <f>I132/D132-1</f>
+        <v>2.6990139052197382E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B133" s="20" t="s">
+        <v>899</v>
+      </c>
+      <c r="D133" s="3">
+        <f>SUMIFS(D$54:D$109,$A$54:$A$109,$B133,$I$54:$I$109,"&gt;0")</f>
+        <v>173566</v>
+      </c>
+      <c r="I133" s="3">
+        <f t="shared" ref="I133:I135" si="19">SUMIFS(I$54:I$109,$A$54:$A$109,$B133,$D$54:$D$109,"&gt;0")</f>
+        <v>176338</v>
+      </c>
+      <c r="J133" s="3">
+        <f t="shared" ref="J133:J136" si="20">I133/D133-1</f>
+        <v>1.5970869870827187E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B134" s="20" t="s">
+        <v>908</v>
+      </c>
+      <c r="D134" s="3">
+        <f>SUMIFS(D$54:D$109,$A$54:$A$109,$B134,$I$54:$I$109,"&gt;0")</f>
+        <v>106878</v>
+      </c>
+      <c r="I134" s="3">
+        <f t="shared" si="19"/>
+        <v>108557</v>
+      </c>
+      <c r="J134" s="3">
+        <f t="shared" si="20"/>
+        <v>1.5709500552031352E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B135" s="20" t="s">
+        <v>907</v>
+      </c>
+      <c r="D135" s="3">
+        <f>SUMIFS(D$54:D$109,$A$54:$A$109,$B135,$I$54:$I$109,"&gt;0")</f>
+        <v>80739</v>
+      </c>
+      <c r="I135" s="3">
+        <f t="shared" si="19"/>
+        <v>82631</v>
+      </c>
+      <c r="J135" s="3">
+        <f t="shared" si="20"/>
+        <v>2.3433532741302221E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B136" s="19" t="s">
+        <v>945</v>
+      </c>
+      <c r="D136" s="3">
+        <f>SUM(D132:D135)</f>
+        <v>937801</v>
+      </c>
+      <c r="I136" s="3">
+        <f>SUM(I132:I135)</f>
+        <v>959707</v>
+      </c>
+      <c r="J136" s="3">
+        <f t="shared" si="20"/>
+        <v>2.3358900235764368E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>